<commit_message>
Added 3^63 -> 1.144561e+30 at 1648537627856
</commit_message>
<xml_diff>
--- a/equations.xlsx
+++ b/equations.xlsx
@@ -418,13 +418,13 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="11.86214285714286" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
     <col width="11.43357142857143" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
@@ -482,6 +482,23 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3^63</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.144561e+30</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1648537627856</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 1953125 -> 1953125 at 1648537964950
</commit_message>
<xml_diff>
--- a/equations.xlsx
+++ b/equations.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,23 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1953125</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1953125</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1648537964950</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 8^9 -> 1.342177e+08 at 1648538283957
</commit_message>
<xml_diff>
--- a/equations.xlsx
+++ b/equations.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,6 +516,23 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>8^9</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1.342177e+08</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1648538283957</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 2^53 -> 9.007199e+15 at 1648538472436
</commit_message>
<xml_diff>
--- a/equations.xlsx
+++ b/equations.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,6 +533,23 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2^53</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>9.007199e+15</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1648538472436</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 2+2 -> 4 at 1648571968260
</commit_message>
<xml_diff>
--- a/equations.xlsx
+++ b/equations.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -45,14 +45,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -134,10 +129,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -175,71 +170,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -267,7 +262,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -290,11 +285,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -303,13 +298,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -319,7 +314,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -328,7 +323,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -337,7 +332,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -345,10 +340,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -421,28 +416,28 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11.86214285714286" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="11.43357142857143" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="13.29071428571429" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="11.85546875" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="21.85546875" customWidth="1" style="1" min="2" max="2"/>
+    <col width="21.140625" customWidth="1" style="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1" s="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Equation</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Eval</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
@@ -502,51 +497,51 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1953125</t>
+          <t>8^9</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1953125</t>
+          <t>1.342177e+08</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1648537964950</t>
+          <t>1648538283957</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>8^9</t>
+          <t>2^53</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.342177e+08</t>
+          <t>9.007199e+15</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1648538283957</t>
+          <t>1648538472436</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2^53</t>
+          <t>2+2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>9.007199e+15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1648538472436</t>
+          <t>1648571968260</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 20% -> NaN at 1650522058298
</commit_message>
<xml_diff>
--- a/equations.xlsx
+++ b/equations.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
@@ -545,6 +545,23 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1650522058298</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>